<commit_message>
presurvey xlsx file is updated
</commit_message>
<xml_diff>
--- a/3_Implementation/presurvey.xlsx
+++ b/3_Implementation/presurvey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ompra\Desktop\sdlcproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638216C5-42B9-47F8-A997-AD72212FEABE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C144ADA-0122-451F-8214-B20A2BFE78C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="2505" windowWidth="15375" windowHeight="7875" xr2:uid="{3DD21051-767B-4BC7-8B26-A6EE86175013}"/>
+    <workbookView xWindow="2850" yWindow="2850" windowWidth="15375" windowHeight="7875" xr2:uid="{3DD21051-767B-4BC7-8B26-A6EE86175013}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>harodharod2017@gmail.com</t>
   </si>
   <si>
-    <t>okankit@gmail.com</t>
-  </si>
-  <si>
     <t>nadarm433@gmail.com</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>chaudharyvidhi16@gmail.com</t>
+  </si>
+  <si>
+    <t>okankit1312@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="A9:I9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -485,22 +485,22 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
       <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -508,7 +508,7 @@
         <v>99003711</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -537,10 +537,10 @@
         <v>99003712</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -566,10 +566,10 @@
         <v>99003713</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -595,10 +595,10 @@
         <v>99003714</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -624,10 +624,10 @@
         <v>99003715</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -653,10 +653,10 @@
         <v>99003716</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -682,10 +682,10 @@
         <v>99003717</v>
       </c>
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -711,10 +711,10 @@
         <v>99003718</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -738,6 +738,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C9" r:id="rId1" xr:uid="{926DE8F6-3DE7-4FA2-AE6C-01C6C848487C}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{88C33186-1A4E-4EE3-854C-11E4B5172598}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>